<commit_message>
added some improvements, deleted some redundent files
</commit_message>
<xml_diff>
--- a/my_project/output_result_data/new_store_best_locations/new_store_best_locations.xlsx
+++ b/my_project/output_result_data/new_store_best_locations/new_store_best_locations.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Total Weighted Demand</t>
+          <t>Score</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -447,1001 +447,1001 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>463.3482272957608</v>
+        <v>463.35</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.527598350697616))</t>
+          <t>(50.436, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>463.3373214866967</v>
+        <v>463.34</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.526598350697615))</t>
+          <t>(50.437, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>463.3214918630744</v>
+        <v>463.32</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.526598350697615))</t>
+          <t>(50.436, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>463.3144127558606</v>
+        <v>463.31</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.527598350697616))</t>
+          <t>(50.437, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>463.28480737464</v>
+        <v>463.28</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.528598350697617))</t>
+          <t>(50.436, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>463.2675009144771</v>
+        <v>463.27</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.525598350697614))</t>
+          <t>(50.437, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>463.2056234337437</v>
+        <v>463.21</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.525598350697614))</t>
+          <t>(50.436, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>463.1981830506404</v>
+        <v>463.2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.528598350697617))</t>
+          <t>(50.437, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>463.191024198144</v>
+        <v>463.19</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.527598350697616))</t>
+          <t>(50.435, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>463.1769271166434</v>
+        <v>463.18</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.528598350697617))</t>
+          <t>(50.435, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>463.1484891341528</v>
+        <v>463.15</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.526598350697615))</t>
+          <t>(50.438, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>463.1298103107949</v>
+        <v>463.13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.52959835069762))</t>
+          <t>(50.436, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>463.126862340295</v>
+        <v>463.13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.525598350697614))</t>
+          <t>(50.438, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>463.1178445705556</v>
+        <v>463.12</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.526598350697615))</t>
+          <t>(50.435, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>463.1051458095831</v>
+        <v>463.11</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.524598350697612))</t>
+          <t>(50.437, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>463.0737175320942</v>
+        <v>463.07</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.52959835069762))</t>
+          <t>(50.435, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>463.0735421603607</v>
+        <v>463.07</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.527598350697616))</t>
+          <t>(50.438, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>463.0084349645243</v>
+        <v>463.01</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.524598350697612))</t>
+          <t>(50.438, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>463.0011153212693</v>
+        <v>463</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.524598350697612))</t>
+          <t>(50.436, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>462.9877534668966</v>
+        <v>462.99</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.52959835069762))</t>
+          <t>(50.437, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>462.958677036292</v>
+        <v>462.96</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.525598350697614))</t>
+          <t>(50.435, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>462.9019767235054</v>
+        <v>462.9</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.528598350697617))</t>
+          <t>(50.438, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>462.8922182204669</v>
+        <v>462.89</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.528598350697617))</t>
+          <t>(50.434, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>462.8815186213949</v>
+        <v>462.88</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.53059835069762))</t>
+          <t>(50.436, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>462.8791522096331</v>
+        <v>462.88</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.53059835069762))</t>
+          <t>(50.435, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>462.8612161545904</v>
+        <v>462.86</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.527598350697616))</t>
+          <t>(50.434, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>462.8499994964018</v>
+        <v>462.85</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.52359835069761))</t>
+          <t>(50.437, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>462.8362746770918</v>
+        <v>462.84</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.52959835069762))</t>
+          <t>(50.434, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>462.7927405749823</v>
+        <v>462.79</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.52359835069761))</t>
+          <t>(50.438, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>462.7696666096203</v>
+        <v>462.77</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.525598350697614))</t>
+          <t>(50.439, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>462.7453389523571</v>
+        <v>462.75</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.526598350697615))</t>
+          <t>(50.434, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>462.7416053170418</v>
+        <v>462.74</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.526598350697615))</t>
+          <t>(50.439, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>462.7141481877754</v>
+        <v>462.71</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.524598350697612))</t>
+          <t>(50.435, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>462.7078432197684</v>
+        <v>462.71</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.52359835069761))</t>
+          <t>(50.436, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>462.6965008254446</v>
+        <v>462.7</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.524598350697612))</t>
+          <t>(50.439, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>462.6907927085322</v>
+        <v>462.69</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.53059835069762))</t>
+          <t>(50.434, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>462.6820185585797</v>
+        <v>462.68</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.53059835069762))</t>
+          <t>(50.437, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>462.6334895791174</v>
+        <v>462.63</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.52959835069762))</t>
+          <t>(50.438, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>462.612953975434</v>
+        <v>462.61</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.527598350697616))</t>
+          <t>(50.439, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>462.590726054073</v>
+        <v>462.59</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.53159835069762))</t>
+          <t>(50.435, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>462.5459938684931</v>
+        <v>462.55</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.525598350697614))</t>
+          <t>(50.434, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>462.5379987990109</v>
+        <v>462.54</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.53159835069762))</t>
+          <t>(50.436, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>462.5214987032122</v>
+        <v>462.52</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.52359835069761))</t>
+          <t>(50.439, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>462.5013482774429</v>
+        <v>462.5</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.52259835069761))</t>
+          <t>(50.437, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>462.4790784348633</v>
+        <v>462.48</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.52259835069761))</t>
+          <t>(50.438, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>462.4528511910613</v>
+        <v>462.45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.53159835069762))</t>
+          <t>(50.434, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>462.4494086614611</v>
+        <v>462.45</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.528598350697617))</t>
+          <t>(50.433, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>462.435754758263</v>
+        <v>462.44</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.52959835069762))</t>
+          <t>(50.433, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>462.3842672904281</v>
+        <v>462.38</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.528598350697617))</t>
+          <t>(50.439, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>462.3841817192577</v>
+        <v>462.38</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.52359835069761))</t>
+          <t>(50.435, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>462.3778677795473</v>
+        <v>462.38</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.527598350697616))</t>
+          <t>(50.433, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>462.3341487317761</v>
+        <v>462.33</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.53059835069762))</t>
+          <t>(50.433, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>462.3250660327998</v>
+        <v>462.33</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.52259835069761))</t>
+          <t>(50.436, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>462.2796957993368</v>
+        <v>462.28</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.53159835069762))</t>
+          <t>(50.437, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>462.2676013360294</v>
+        <v>462.27</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.53059835069762))</t>
+          <t>(50.438, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>462.2638566201961</v>
+        <v>462.26</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.524598350697612))</t>
+          <t>(50.434, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>462.2439940663283</v>
+        <v>462.24</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.52259835069761))</t>
+          <t>(50.439, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>462.2232937909966</v>
+        <v>462.22</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.526598350697615))</t>
+          <t>(50.433, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>462.2058422157297</v>
+        <v>462.21</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.532598350697622))</t>
+          <t>(50.435, 30.533)</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>462.185445094464</v>
+        <v>462.19</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.525598350697614))</t>
+          <t>(50.44, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>462.1589544912089</v>
+        <v>462.16</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.524598350697612))</t>
+          <t>(50.44, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>462.1414550336118</v>
+        <v>462.14</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.53159835069762))</t>
+          <t>(50.433, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>462.1194464887499</v>
+        <v>462.12</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.532598350697622))</t>
+          <t>(50.434, 30.533)</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>462.1064577830566</v>
+        <v>462.11</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.526598350697615))</t>
+          <t>(50.44, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>462.0971987736244</v>
+        <v>462.1</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.532598350697622))</t>
+          <t>(50.436, 30.533)</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>462.0664477810514</v>
+        <v>462.07</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.52159835069761))</t>
+          <t>(50.438, 30.522)</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>462.0580162092202</v>
+        <v>462.06</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.52159835069761))</t>
+          <t>(50.437, 30.522)</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>462.0559047889798</v>
+        <v>462.06</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.52959835069762))</t>
+          <t>(50.439, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>462.0262543643785</v>
+        <v>462.03</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.52359835069761))</t>
+          <t>(50.44, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>461.9871314422055</v>
+        <v>461.99</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.525598350697614))</t>
+          <t>(50.433, 30.526)</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>461.968013735744</v>
+        <v>461.97</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.52259835069761))</t>
+          <t>(50.435, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>461.9229485038982</v>
+        <v>461.92</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.527598350697616))</t>
+          <t>(50.44, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>461.8988551832433</v>
+        <v>461.9</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.52359835069761))</t>
+          <t>(50.434, 30.524)</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>461.8905814131826</v>
+        <v>461.89</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.52959835069762))</t>
+          <t>(50.432, 30.53)</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>461.8668649109264</v>
+        <v>461.87</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.528598350697617))</t>
+          <t>(50.432, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>461.8631884644786</v>
+        <v>461.86</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.52159835069761))</t>
+          <t>(50.439, 30.522)</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>461.8545172144944</v>
+        <v>461.85</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.532598350697622))</t>
+          <t>(50.433, 30.533)</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>461.8514722402967</v>
+        <v>461.85</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.52159835069761))</t>
+          <t>(50.436, 30.522)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>461.827673986749</v>
+        <v>461.83</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.53059835069762))</t>
+          <t>(50.432, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>461.8037558953288</v>
+        <v>461.8</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.53159835069762))</t>
+          <t>(50.438, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>461.7867887242045</v>
+        <v>461.79</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.52259835069761))</t>
+          <t>(50.44, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>461.7793913499635</v>
+        <v>461.78</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.532598350697622))</t>
+          <t>(50.437, 30.533)</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>461.759276871944</v>
+        <v>461.76</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.527598350697616))</t>
+          <t>(50.432, 30.528)</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>461.722122730258</v>
+        <v>461.72</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.533598350697623))</t>
+          <t>(50.435, 30.534)</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>461.6879017387776</v>
+        <v>461.69</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.533598350697623))</t>
+          <t>(50.434, 30.534)</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>461.6750235478201</v>
+        <v>461.68</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.53159835069762))</t>
+          <t>(50.432, 30.532)</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>461.6700579361346</v>
+        <v>461.67</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.524598350697612))</t>
+          <t>(50.433, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>461.6360048138135</v>
+        <v>461.64</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.528598350697617))</t>
+          <t>(50.44, 30.529)</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>461.6281109893264</v>
+        <v>461.63</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.53059835069762))</t>
+          <t>(50.439, 30.531)</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>461.5699734800775</v>
+        <v>461.57</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.526598350697615))</t>
+          <t>(50.432, 30.527)</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>461.5571807959006</v>
+        <v>461.56</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>(np.float64(50.43646254621184), np.float64(30.533598350697623))</t>
+          <t>(50.436, 30.534)</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>461.5536141565265</v>
+        <v>461.55</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>(np.float64(50.43846254621184), np.float64(30.520598350697608))</t>
+          <t>(50.438, 30.521)</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>461.5184453360325</v>
+        <v>461.52</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>(np.float64(50.43746254621184), np.float64(30.520598350697608))</t>
+          <t>(50.437, 30.521)</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>461.470433978233</v>
+        <v>461.47</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>(np.float64(50.43346254621185), np.float64(30.533598350697623))</t>
+          <t>(50.433, 30.534)</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>461.464260220763</v>
+        <v>461.46</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>(np.float64(50.435462546211845), np.float64(30.52159835069761))</t>
+          <t>(50.435, 30.522)</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>461.4502062368932</v>
+        <v>461.45</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>(np.float64(50.43446254621185), np.float64(30.52259835069761))</t>
+          <t>(50.434, 30.523)</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>461.4401397563369</v>
+        <v>461.44</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>(np.float64(50.44046254621183), np.float64(30.52159835069761))</t>
+          <t>(50.44, 30.522)</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>461.4293623810377</v>
+        <v>461.43</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>(np.float64(50.43246254621185), np.float64(30.532598350697622))</t>
+          <t>(50.432, 30.533)</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>461.3909084137235</v>
+        <v>461.39</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>(np.float64(50.44146254621183), np.float64(30.524598350697612))</t>
+          <t>(50.441, 30.525)</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>461.3783120084034</v>
+        <v>461.38</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>(np.float64(50.439462546211836), np.float64(30.520598350697608))</t>
+          <t>(50.439, 30.521)</t>
         </is>
       </c>
     </row>

</xml_diff>